<commit_message>
Added the variable FEF75_z_
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abz_r\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E143C96-4D9C-F74E-A885-ABFA301722B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A85297-2DF9-4F49-B519-54FE2FA9F16A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2800" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="305">
   <si>
     <t>name</t>
   </si>
@@ -930,17 +930,30 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>FEF75_z_</t>
+  </si>
+  <si>
+    <t>FEF75 (z-score according to GLI)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -971,6 +984,11 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1031,32 +1049,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{EAC5DA9D-1B7A-46C8-A38C-E194DDCBDEDD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1515,21 +1542,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG107"/>
+  <dimension ref="A1:BG108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="15.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="29.1796875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="15.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1625,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1612,7 +1639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1624,7 +1651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -1638,7 +1665,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1653,7 +1680,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1668,7 +1695,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1683,7 +1710,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -1698,7 +1725,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1713,7 +1740,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1728,7 +1755,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -1742,7 +1769,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
@@ -1756,7 +1783,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -1770,7 +1797,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -1784,7 +1811,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -1798,7 +1825,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
@@ -1812,7 +1839,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>50</v>
       </c>
@@ -1826,7 +1853,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>52</v>
       </c>
@@ -1840,23 +1867,23 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>5</v>
@@ -1865,40 +1892,40 @@
         <v>6</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -1907,12 +1934,12 @@
         <v>6</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>5</v>
@@ -1921,12 +1948,12 @@
         <v>6</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>5</v>
@@ -1935,12 +1962,12 @@
         <v>6</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>5</v>
@@ -1949,26 +1976,26 @@
         <v>6</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -1977,54 +2004,54 @@
         <v>17</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>80</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>5</v>
@@ -2033,68 +2060,68 @@
         <v>6</v>
       </c>
       <c r="D32" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="C34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="B35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="B36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>91</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>5</v>
@@ -2103,96 +2130,96 @@
         <v>6</v>
       </c>
       <c r="D37" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="11" t="s">
+      <c r="B39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="11" t="s">
+      <c r="B40" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="B41" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="11" t="s">
+      <c r="B42" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="11" t="s">
+      <c r="B43" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>5</v>
@@ -2201,96 +2228,96 @@
         <v>6</v>
       </c>
       <c r="D44" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="11" t="s">
+      <c r="B46" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="11" t="s">
+      <c r="B47" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B47" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="11" t="s">
+      <c r="B48" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="11" t="s">
+      <c r="B49" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="11" t="s">
+      <c r="B50" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>5</v>
@@ -2299,138 +2326,138 @@
         <v>6</v>
       </c>
       <c r="D51" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="11" t="s">
+      <c r="B53" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B53" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="11" t="s">
+      <c r="B54" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="11" t="s">
+      <c r="B55" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B56" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="11" t="s">
+      <c r="C56" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B56" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="11" t="s">
+      <c r="B57" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D57" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B58" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="11" t="s">
+      <c r="C58" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B58" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="11" t="s">
+      <c r="B59" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C59" s="11" t="s">
+      <c r="B60" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D60" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="11" t="s">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="11" t="s">
-        <v>139</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>5</v>
@@ -2439,138 +2466,138 @@
         <v>6</v>
       </c>
       <c r="D61" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="11" t="s">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="11" t="s">
+      <c r="B63" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="11" t="s">
+      <c r="B64" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="B64" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="11" t="s">
+      <c r="B65" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B66" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="11" t="s">
+      <c r="C66" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="11" t="s">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="11" t="s">
+      <c r="B67" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D67" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="11" t="s">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B68" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="11" t="s">
+      <c r="C68" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="11" t="s">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="11" t="s">
+      <c r="B69" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C69" s="11" t="s">
+      <c r="B70" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D70" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="11" t="s">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>5</v>
@@ -2579,110 +2606,110 @@
         <v>6</v>
       </c>
       <c r="D71" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="11" t="s">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="11" t="s">
+      <c r="B73" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="11" t="s">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B73" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" s="11" t="s">
+      <c r="B74" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="11" t="s">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="B74" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" s="11" t="s">
+      <c r="B75" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="11" t="s">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B75" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="11" t="s">
+      <c r="B76" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="11" t="s">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="B76" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="11" t="s">
+      <c r="B77" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="11" t="s">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B77" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C77" s="11" t="s">
+      <c r="B78" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D78" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="11" t="s">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="11" t="s">
         <v>173</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="11" t="s">
-        <v>175</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>5</v>
@@ -2691,110 +2718,110 @@
         <v>6</v>
       </c>
       <c r="D79" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="11" t="s">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B80" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="11" t="s">
+      <c r="B81" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="11" t="s">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="B81" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="11" t="s">
+      <c r="B82" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="11" t="s">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="B82" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="11" t="s">
+      <c r="B83" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="11" t="s">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B83" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="11" t="s">
+      <c r="B84" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="11" t="s">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="11" t="s">
+      <c r="B85" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="11" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="11" t="s">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B85" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C85" s="11" t="s">
+      <c r="B86" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="11" t="s">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="11" t="s">
-        <v>191</v>
       </c>
       <c r="B87" s="11" t="s">
         <v>5</v>
@@ -2803,110 +2830,110 @@
         <v>6</v>
       </c>
       <c r="D87" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="11" t="s">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B88" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" s="11" t="s">
+      <c r="B89" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="11" t="s">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B89" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="11" t="s">
+      <c r="B90" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="11" t="s">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="B90" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="11" t="s">
+      <c r="B91" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="11" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="11" t="s">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="B91" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="11" t="s">
+      <c r="B92" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="11" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="11" t="s">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B92" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C92" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92" s="11" t="s">
+      <c r="B93" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="11" t="s">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B93" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C93" s="11" t="s">
+      <c r="B94" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="D94" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="11" t="s">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="11" t="s">
         <v>205</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="B95" s="11" t="s">
         <v>5</v>
@@ -2915,110 +2942,110 @@
         <v>6</v>
       </c>
       <c r="D95" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="11" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="11" t="s">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B96" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C96" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" s="11" t="s">
+      <c r="B97" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="11" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="11" t="s">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B97" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C97" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D97" s="11" t="s">
+      <c r="B98" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="11" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="11" t="s">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="B98" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C98" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" s="11" t="s">
+      <c r="B99" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="11" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="11" t="s">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="B99" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D99" s="11" t="s">
+      <c r="B100" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="11" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="11" t="s">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="B100" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C100" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D100" s="11" t="s">
+      <c r="B101" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="11" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="11" t="s">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B101" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C101" s="11" t="s">
+      <c r="B102" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D101" s="11" t="s">
+      <c r="D102" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="11" t="s">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="11" t="s">
         <v>221</v>
-      </c>
-      <c r="B102" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D102" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="11" t="s">
-        <v>223</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>5</v>
@@ -3027,67 +3054,81 @@
         <v>6</v>
       </c>
       <c r="D103" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="11" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="11" t="s">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B104" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D104" s="11" t="s">
+      <c r="B105" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="11" t="s">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B105" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C105" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D105" s="11" t="s">
+      <c r="B106" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" s="11" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="11" t="s">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="B106" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C106" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" s="11" t="s">
+      <c r="B107" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="11" t="s">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B107" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" s="11" t="s">
+      <c r="B108" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="11" t="s">
         <v>232</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="2048"/>
   <headerFooter alignWithMargins="0">
@@ -3104,14 +3145,14 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="37.36328125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="18.453125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -3125,7 +3166,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -3139,7 +3180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -3153,7 +3194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -3167,7 +3208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -3181,7 +3222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -3195,7 +3236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -3209,7 +3250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -3223,7 +3264,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -3237,7 +3278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -3251,7 +3292,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3265,7 +3306,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -3279,7 +3320,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -3293,7 +3334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -3307,7 +3348,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -3321,7 +3362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -3335,7 +3376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>54</v>
       </c>
@@ -3349,7 +3390,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>54</v>
       </c>
@@ -3363,7 +3404,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -3377,7 +3418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -3391,7 +3432,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>60</v>
       </c>
@@ -3405,7 +3446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>60</v>
       </c>
@@ -3419,7 +3460,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -3433,7 +3474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
@@ -3447,7 +3488,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>64</v>
       </c>
@@ -3461,7 +3502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>64</v>
       </c>
@@ -3475,7 +3516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
@@ -3489,7 +3530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>66</v>
       </c>
@@ -3503,7 +3544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
@@ -3517,7 +3558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>68</v>
       </c>
@@ -3531,7 +3572,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
@@ -3545,7 +3586,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>91</v>
       </c>
@@ -3559,7 +3600,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>91</v>
       </c>
@@ -3573,7 +3614,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>91</v>
       </c>
@@ -3587,7 +3628,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>91</v>
       </c>
@@ -3601,7 +3642,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>91</v>
       </c>
@@ -3615,7 +3656,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>89</v>
       </c>
@@ -3629,7 +3670,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>89</v>
       </c>
@@ -3643,7 +3684,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>89</v>
       </c>
@@ -3657,7 +3698,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>89</v>
       </c>
@@ -3671,7 +3712,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>89</v>
       </c>
@@ -3685,7 +3726,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>89</v>
       </c>
@@ -3699,7 +3740,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>105</v>
       </c>
@@ -3713,7 +3754,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>105</v>
       </c>
@@ -3727,7 +3768,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>105</v>
       </c>
@@ -3741,7 +3782,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>105</v>
       </c>
@@ -3755,7 +3796,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>105</v>
       </c>
@@ -3769,7 +3810,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>105</v>
       </c>
@@ -3783,7 +3824,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>103</v>
       </c>
@@ -3797,7 +3838,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>103</v>
       </c>
@@ -3811,7 +3852,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>103</v>
       </c>
@@ -3825,7 +3866,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>103</v>
       </c>
@@ -3839,7 +3880,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>103</v>
       </c>
@@ -3853,7 +3894,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>103</v>
       </c>
@@ -3867,7 +3908,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>119</v>
       </c>
@@ -3881,7 +3922,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
@@ -3895,7 +3936,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>119</v>
       </c>
@@ -3909,7 +3950,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>119</v>
       </c>
@@ -3923,7 +3964,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>119</v>
       </c>
@@ -3937,7 +3978,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>119</v>
       </c>
@@ -3951,7 +3992,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>117</v>
       </c>
@@ -3965,7 +4006,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>117</v>
       </c>
@@ -3979,7 +4020,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>117</v>
       </c>
@@ -3993,7 +4034,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>117</v>
       </c>
@@ -4007,7 +4048,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>117</v>
       </c>
@@ -4021,7 +4062,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>127</v>
       </c>
@@ -4035,7 +4076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>127</v>
       </c>
@@ -4049,7 +4090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>131</v>
       </c>
@@ -4063,7 +4104,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>131</v>
       </c>
@@ -4077,7 +4118,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>139</v>
       </c>
@@ -4091,7 +4132,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>139</v>
       </c>
@@ -4105,7 +4146,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>139</v>
       </c>
@@ -4119,7 +4160,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>139</v>
       </c>
@@ -4133,7 +4174,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>139</v>
       </c>
@@ -4147,7 +4188,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>139</v>
       </c>
@@ -4161,7 +4202,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>137</v>
       </c>
@@ -4175,7 +4216,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>137</v>
       </c>
@@ -4189,7 +4230,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>137</v>
       </c>
@@ -4203,7 +4244,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>137</v>
       </c>
@@ -4217,7 +4258,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>137</v>
       </c>
@@ -4231,7 +4272,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>137</v>
       </c>
@@ -4245,7 +4286,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>137</v>
       </c>
@@ -4259,7 +4300,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>137</v>
       </c>
@@ -4273,7 +4314,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>147</v>
       </c>
@@ -4287,7 +4328,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>147</v>
       </c>
@@ -4301,7 +4342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>151</v>
       </c>
@@ -4315,7 +4356,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>151</v>
       </c>
@@ -4329,7 +4370,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>159</v>
       </c>
@@ -4343,7 +4384,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>159</v>
       </c>
@@ -4357,7 +4398,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>159</v>
       </c>
@@ -4371,7 +4412,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>159</v>
       </c>
@@ -4385,7 +4426,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>159</v>
       </c>
@@ -4399,7 +4440,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>159</v>
       </c>
@@ -4413,7 +4454,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>157</v>
       </c>
@@ -4427,7 +4468,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>157</v>
       </c>
@@ -4441,7 +4482,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>157</v>
       </c>
@@ -4455,7 +4496,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>157</v>
       </c>
@@ -4469,7 +4510,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>157</v>
       </c>
@@ -4483,7 +4524,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>157</v>
       </c>
@@ -4497,7 +4538,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>157</v>
       </c>
@@ -4511,7 +4552,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>157</v>
       </c>
@@ -4525,7 +4566,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
         <v>157</v>
       </c>
@@ -4539,7 +4580,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>157</v>
       </c>
@@ -4553,7 +4594,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>157</v>
       </c>
@@ -4567,7 +4608,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>157</v>
       </c>
@@ -4581,7 +4622,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>157</v>
       </c>
@@ -4595,7 +4636,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
         <v>157</v>
       </c>
@@ -4609,7 +4650,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
         <v>175</v>
       </c>
@@ -4623,7 +4664,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>175</v>
       </c>
@@ -4637,7 +4678,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>175</v>
       </c>
@@ -4651,7 +4692,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>175</v>
       </c>
@@ -4665,7 +4706,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>175</v>
       </c>
@@ -4679,7 +4720,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
         <v>175</v>
       </c>
@@ -4693,7 +4734,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>173</v>
       </c>
@@ -4707,7 +4748,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>173</v>
       </c>
@@ -4721,7 +4762,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>173</v>
       </c>
@@ -4735,7 +4776,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>173</v>
       </c>
@@ -4749,7 +4790,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>173</v>
       </c>
@@ -4763,7 +4804,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>173</v>
       </c>
@@ -4777,7 +4818,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>173</v>
       </c>
@@ -4791,7 +4832,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>173</v>
       </c>
@@ -4805,7 +4846,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>173</v>
       </c>
@@ -4819,7 +4860,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>173</v>
       </c>
@@ -4833,7 +4874,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>173</v>
       </c>
@@ -4847,7 +4888,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>173</v>
       </c>
@@ -4861,7 +4902,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>173</v>
       </c>
@@ -4875,7 +4916,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>173</v>
       </c>
@@ -4889,7 +4930,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>173</v>
       </c>
@@ -4903,7 +4944,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>173</v>
       </c>
@@ -4917,7 +4958,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>173</v>
       </c>
@@ -4931,7 +4972,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="s">
         <v>191</v>
       </c>
@@ -4945,7 +4986,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>191</v>
       </c>
@@ -4959,7 +5000,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>191</v>
       </c>
@@ -4973,7 +5014,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>191</v>
       </c>
@@ -4987,7 +5028,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>191</v>
       </c>
@@ -5001,7 +5042,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>191</v>
       </c>
@@ -5015,7 +5056,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>189</v>
       </c>
@@ -5029,7 +5070,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>189</v>
       </c>
@@ -5043,7 +5084,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>189</v>
       </c>
@@ -5057,7 +5098,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>189</v>
       </c>
@@ -5071,7 +5112,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>189</v>
       </c>
@@ -5085,7 +5126,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>189</v>
       </c>
@@ -5099,7 +5140,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
         <v>189</v>
       </c>
@@ -5113,7 +5154,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="4" t="s">
         <v>189</v>
       </c>
@@ -5127,7 +5168,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
         <v>189</v>
       </c>
@@ -5141,7 +5182,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" s="4" t="s">
         <v>189</v>
       </c>
@@ -5155,7 +5196,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="4" t="s">
         <v>189</v>
       </c>
@@ -5169,7 +5210,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="4" t="s">
         <v>189</v>
       </c>
@@ -5183,7 +5224,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
         <v>189</v>
       </c>
@@ -5197,7 +5238,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="4" t="s">
         <v>189</v>
       </c>
@@ -5211,7 +5252,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
         <v>207</v>
       </c>
@@ -5225,7 +5266,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="4" t="s">
         <v>207</v>
       </c>
@@ -5239,7 +5280,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
         <v>207</v>
       </c>
@@ -5253,7 +5294,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" s="4" t="s">
         <v>207</v>
       </c>
@@ -5267,7 +5308,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" s="4" t="s">
         <v>207</v>
       </c>
@@ -5281,7 +5322,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="4" t="s">
         <v>207</v>
       </c>
@@ -5295,7 +5336,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" s="4" t="s">
         <v>205</v>
       </c>
@@ -5309,7 +5350,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
         <v>205</v>
       </c>
@@ -5323,7 +5364,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
         <v>223</v>
       </c>
@@ -5337,7 +5378,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
         <v>223</v>
       </c>
@@ -5351,7 +5392,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
         <v>223</v>
       </c>
@@ -5365,7 +5406,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="4" t="s">
         <v>223</v>
       </c>
@@ -5379,7 +5420,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="4" t="s">
         <v>223</v>
       </c>
@@ -5393,7 +5434,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>223</v>
       </c>
@@ -5407,7 +5448,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="4" t="s">
         <v>221</v>
       </c>
@@ -5421,7 +5462,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
         <v>221</v>
       </c>
@@ -5435,7 +5476,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="4" t="s">
         <v>221</v>
       </c>
@@ -5449,7 +5490,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>221</v>
       </c>
@@ -5463,7 +5504,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="4" t="s">
         <v>221</v>
       </c>
@@ -5477,7 +5518,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
         <v>221</v>
       </c>
@@ -5491,7 +5532,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="4" t="s">
         <v>221</v>
       </c>
@@ -5505,7 +5546,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
         <v>221</v>
       </c>
@@ -5519,7 +5560,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="4" t="s">
         <v>221</v>
       </c>
@@ -5533,7 +5574,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
         <v>221</v>
       </c>
@@ -5547,7 +5588,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="4" t="s">
         <v>221</v>
       </c>
@@ -5561,7 +5602,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
         <v>221</v>
       </c>
@@ -5575,7 +5616,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="4" t="s">
         <v>221</v>
       </c>
@@ -5589,7 +5630,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="4" t="s">
         <v>221</v>
       </c>
@@ -5603,7 +5644,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
         <v>221</v>
       </c>
@@ -5617,7 +5658,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="4" t="s">
         <v>221</v>
       </c>
@@ -5631,7 +5672,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="4" t="s">
         <v>221</v>
       </c>
@@ -5645,7 +5686,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="4" t="s">
         <v>221</v>
       </c>
@@ -5659,7 +5700,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="4" t="s">
         <v>221</v>
       </c>
@@ -5673,7 +5714,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="4" t="s">
         <v>221</v>
       </c>
@@ -5687,7 +5728,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="4" t="s">
         <v>221</v>
       </c>
@@ -5701,7 +5742,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="4" t="s">
         <v>221</v>
       </c>
@@ -5715,7 +5756,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="4" t="s">
         <v>221</v>
       </c>
@@ -5729,7 +5770,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="4" t="s">
         <v>221</v>
       </c>
@@ -5743,7 +5784,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="4" t="s">
         <v>221</v>
       </c>
@@ -5757,7 +5798,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="4" t="s">
         <v>221</v>
       </c>
@@ -5771,7 +5812,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="4" t="s">
         <v>221</v>
       </c>
@@ -5785,7 +5826,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="4" t="s">
         <v>221</v>
       </c>
@@ -5799,7 +5840,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="4" t="s">
         <v>221</v>
       </c>
@@ -5813,7 +5854,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" s="4" t="s">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
fix: remove carage returns
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abz_r\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C517EB-8661-41A2-90F7-6865BB807970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DEDDF1-4862-5C42-8A86-AD419A4A615D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="355">
   <si>
     <t>name</t>
   </si>
@@ -1077,6 +1077,21 @@
   </si>
   <si>
     <t>food_all_sens_SPT_WHEAT_</t>
+  </si>
+  <si>
+    <t>food_all_sens_SPT_NUT_mix_</t>
+  </si>
+  <si>
+    <t>food_all_sens_SPT_NUT_wal_</t>
+  </si>
+  <si>
+    <t>food_all_sens_SPT_NUT_haz_</t>
+  </si>
+  <si>
+    <t>food_all_sens_SPT_SES_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_HDM_mix _</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1219,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1219,21 +1234,15 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1700,19 +1709,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A98" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108:D130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="15.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="97.90625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="97.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1781,7 +1790,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1807,7 +1816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -1821,7 +1830,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1836,7 +1845,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1851,7 +1860,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1866,7 +1875,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -1881,7 +1890,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1896,7 +1905,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1911,7 +1920,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -1925,7 +1934,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
@@ -1939,7 +1948,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -1953,7 +1962,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -1967,7 +1976,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -1981,7 +1990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>50</v>
       </c>
@@ -2009,7 +2018,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>52</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>54</v>
       </c>
@@ -2037,7 +2046,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
@@ -2065,7 +2074,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>60</v>
       </c>
@@ -2079,7 +2088,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -2093,7 +2102,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>64</v>
       </c>
@@ -2107,7 +2116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>66</v>
       </c>
@@ -2121,7 +2130,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>68</v>
       </c>
@@ -2135,7 +2144,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>71</v>
       </c>
@@ -2149,7 +2158,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>73</v>
       </c>
@@ -2163,7 +2172,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>74</v>
       </c>
@@ -2177,7 +2186,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>76</v>
       </c>
@@ -2191,7 +2200,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>78</v>
       </c>
@@ -2205,7 +2214,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>80</v>
       </c>
@@ -2219,7 +2228,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>82</v>
       </c>
@@ -2233,7 +2242,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>84</v>
       </c>
@@ -2247,7 +2256,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>86</v>
       </c>
@@ -2261,7 +2270,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>89</v>
       </c>
@@ -2275,7 +2284,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>91</v>
       </c>
@@ -2289,7 +2298,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>93</v>
       </c>
@@ -2303,7 +2312,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>95</v>
       </c>
@@ -2317,7 +2326,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>97</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>99</v>
       </c>
@@ -2345,7 +2354,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>101</v>
       </c>
@@ -2359,7 +2368,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>103</v>
       </c>
@@ -2373,7 +2382,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>105</v>
       </c>
@@ -2387,7 +2396,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>107</v>
       </c>
@@ -2401,7 +2410,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>109</v>
       </c>
@@ -2415,7 +2424,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>111</v>
       </c>
@@ -2429,7 +2438,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>113</v>
       </c>
@@ -2443,7 +2452,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>115</v>
       </c>
@@ -2457,7 +2466,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>117</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>119</v>
       </c>
@@ -2485,7 +2494,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>121</v>
       </c>
@@ -2499,7 +2508,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>123</v>
       </c>
@@ -2513,7 +2522,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>125</v>
       </c>
@@ -2527,7 +2536,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>127</v>
       </c>
@@ -2541,7 +2550,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>129</v>
       </c>
@@ -2555,7 +2564,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>131</v>
       </c>
@@ -2569,7 +2578,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>133</v>
       </c>
@@ -2583,7 +2592,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>135</v>
       </c>
@@ -2597,7 +2606,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>137</v>
       </c>
@@ -2611,7 +2620,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>139</v>
       </c>
@@ -2625,7 +2634,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>141</v>
       </c>
@@ -2639,7 +2648,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
         <v>143</v>
       </c>
@@ -2653,7 +2662,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>145</v>
       </c>
@@ -2667,7 +2676,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>147</v>
       </c>
@@ -2681,7 +2690,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>149</v>
       </c>
@@ -2695,7 +2704,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
         <v>151</v>
       </c>
@@ -2709,7 +2718,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>153</v>
       </c>
@@ -2723,7 +2732,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>155</v>
       </c>
@@ -2737,7 +2746,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>157</v>
       </c>
@@ -2751,7 +2760,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>159</v>
       </c>
@@ -2765,7 +2774,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
         <v>161</v>
       </c>
@@ -2779,7 +2788,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>163</v>
       </c>
@@ -2793,7 +2802,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
         <v>165</v>
       </c>
@@ -2807,7 +2816,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
         <v>167</v>
       </c>
@@ -2821,7 +2830,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
         <v>169</v>
       </c>
@@ -2835,7 +2844,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>171</v>
       </c>
@@ -2849,7 +2858,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
         <v>173</v>
       </c>
@@ -2863,7 +2872,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
         <v>175</v>
       </c>
@@ -2877,7 +2886,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
         <v>177</v>
       </c>
@@ -2891,7 +2900,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>179</v>
       </c>
@@ -2905,7 +2914,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
         <v>181</v>
       </c>
@@ -2919,7 +2928,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>183</v>
       </c>
@@ -2933,7 +2942,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
         <v>185</v>
       </c>
@@ -2947,7 +2956,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>187</v>
       </c>
@@ -2961,7 +2970,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
         <v>189</v>
       </c>
@@ -2975,7 +2984,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>191</v>
       </c>
@@ -2989,7 +2998,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
         <v>193</v>
       </c>
@@ -3003,7 +3012,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>195</v>
       </c>
@@ -3017,7 +3026,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
         <v>197</v>
       </c>
@@ -3031,7 +3040,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>199</v>
       </c>
@@ -3045,7 +3054,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
         <v>201</v>
       </c>
@@ -3059,7 +3068,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
         <v>203</v>
       </c>
@@ -3073,7 +3082,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
         <v>205</v>
       </c>
@@ -3087,7 +3096,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>207</v>
       </c>
@@ -3101,7 +3110,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
         <v>209</v>
       </c>
@@ -3115,7 +3124,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
         <v>211</v>
       </c>
@@ -3129,7 +3138,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
         <v>213</v>
       </c>
@@ -3143,7 +3152,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
         <v>215</v>
       </c>
@@ -3157,7 +3166,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
         <v>217</v>
       </c>
@@ -3171,7 +3180,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
         <v>219</v>
       </c>
@@ -3185,7 +3194,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
         <v>221</v>
       </c>
@@ -3199,7 +3208,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
         <v>223</v>
       </c>
@@ -3213,7 +3222,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
         <v>225</v>
       </c>
@@ -3227,7 +3236,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
         <v>227</v>
       </c>
@@ -3241,7 +3250,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
         <v>229</v>
       </c>
@@ -3255,7 +3264,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="13" t="s">
         <v>231</v>
       </c>
@@ -3269,325 +3278,325 @@
         <v>232</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="14" t="s">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>303</v>
       </c>
-      <c r="B108" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D108" s="16" t="s">
+      <c r="B108" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="14" t="s">
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>305</v>
       </c>
-      <c r="B109" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" s="16" t="s">
+      <c r="B109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="B110" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D110" s="16" t="s">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="14" t="s">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>309</v>
       </c>
-      <c r="B111" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" s="16" t="s">
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="B112" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D112" s="16" t="s">
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>350</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="B113" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D113" s="16" t="s">
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>351</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="14" t="s">
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>315</v>
       </c>
-      <c r="B114" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D114" s="16" t="s">
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D115" s="16" t="s">
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>352</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="B116" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D116" s="16" t="s">
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>353</v>
+      </c>
+      <c r="B116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="14" t="s">
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>321</v>
       </c>
-      <c r="B117" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C117" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="16" t="s">
+      <c r="B117" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="14" t="s">
+    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>323</v>
       </c>
-      <c r="B118" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C118" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D118" s="16" t="s">
+      <c r="B118" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="14" t="s">
+    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>325</v>
       </c>
-      <c r="B119" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D119" s="16" t="s">
+      <c r="B119" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="14" t="s">
+    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>327</v>
       </c>
-      <c r="B120" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C120" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D120" s="16" t="s">
+      <c r="B120" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="14" t="s">
+    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>329</v>
       </c>
-      <c r="B121" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C121" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D121" s="16" t="s">
+      <c r="B121" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="14" t="s">
+    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>331</v>
       </c>
-      <c r="B122" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C122" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" s="16" t="s">
+      <c r="B122" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="14" t="s">
+    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>333</v>
       </c>
-      <c r="B123" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C123" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D123" s="16" t="s">
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="14" t="s">
+    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>335</v>
       </c>
-      <c r="B124" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C124" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D124" s="16" t="s">
+      <c r="B124" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124" t="s">
+        <v>6</v>
+      </c>
+      <c r="D124" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="14" t="s">
+    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>337</v>
       </c>
-      <c r="B125" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C125" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D125" s="16" t="s">
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="B126" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C126" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D126" s="16" t="s">
+    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>354</v>
+      </c>
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="14" t="s">
+    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>341</v>
       </c>
-      <c r="B127" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C127" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D127" s="14" t="s">
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="14" t="s">
+    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>343</v>
       </c>
-      <c r="B128" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C128" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D128" s="14" t="s">
+      <c r="B128" t="s">
+        <v>5</v>
+      </c>
+      <c r="C128" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="14" t="s">
+    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>345</v>
       </c>
-      <c r="B129" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C129" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D129" s="16" t="s">
+      <c r="B129" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129" t="s">
+        <v>6</v>
+      </c>
+      <c r="D129" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="14" t="s">
+    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>347</v>
       </c>
-      <c r="B130" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C130" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D130" s="16" t="s">
+      <c r="B130" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" t="s">
         <v>348</v>
       </c>
     </row>
@@ -3609,14 +3618,14 @@
       <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.36328125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="18.453125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="18.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -3630,7 +3639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -3644,7 +3653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -3658,7 +3667,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -3672,7 +3681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -3686,7 +3695,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -3700,7 +3709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -3714,7 +3723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -3728,7 +3737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -3742,7 +3751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -3756,7 +3765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3770,7 +3779,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -3784,7 +3793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -3798,7 +3807,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -3812,7 +3821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -3840,7 +3849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>54</v>
       </c>
@@ -3854,7 +3863,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>54</v>
       </c>
@@ -3868,7 +3877,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -3882,7 +3891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -3896,7 +3905,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>60</v>
       </c>
@@ -3910,7 +3919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>60</v>
       </c>
@@ -3924,7 +3933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -3938,7 +3947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
@@ -3952,7 +3961,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>64</v>
       </c>
@@ -3966,7 +3975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>64</v>
       </c>
@@ -3980,7 +3989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
@@ -3994,7 +4003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>66</v>
       </c>
@@ -4008,7 +4017,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
@@ -4022,7 +4031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>68</v>
       </c>
@@ -4036,7 +4045,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>91</v>
       </c>
@@ -4050,7 +4059,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>91</v>
       </c>
@@ -4064,7 +4073,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>91</v>
       </c>
@@ -4078,7 +4087,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>91</v>
       </c>
@@ -4092,7 +4101,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>91</v>
       </c>
@@ -4106,7 +4115,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>91</v>
       </c>
@@ -4120,7 +4129,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>89</v>
       </c>
@@ -4134,7 +4143,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>89</v>
       </c>
@@ -4148,7 +4157,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>89</v>
       </c>
@@ -4162,7 +4171,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>89</v>
       </c>
@@ -4176,7 +4185,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>89</v>
       </c>
@@ -4190,7 +4199,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>89</v>
       </c>
@@ -4204,7 +4213,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>105</v>
       </c>
@@ -4218,7 +4227,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>105</v>
       </c>
@@ -4232,7 +4241,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>105</v>
       </c>
@@ -4246,7 +4255,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>105</v>
       </c>
@@ -4260,7 +4269,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>105</v>
       </c>
@@ -4274,7 +4283,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>105</v>
       </c>
@@ -4288,7 +4297,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>103</v>
       </c>
@@ -4302,7 +4311,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>103</v>
       </c>
@@ -4316,7 +4325,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>103</v>
       </c>
@@ -4330,7 +4339,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>103</v>
       </c>
@@ -4344,7 +4353,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>103</v>
       </c>
@@ -4358,7 +4367,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>103</v>
       </c>
@@ -4372,7 +4381,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>119</v>
       </c>
@@ -4386,7 +4395,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
@@ -4400,7 +4409,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>119</v>
       </c>
@@ -4414,7 +4423,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>119</v>
       </c>
@@ -4428,7 +4437,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>119</v>
       </c>
@@ -4442,7 +4451,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>119</v>
       </c>
@@ -4456,7 +4465,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>117</v>
       </c>
@@ -4470,7 +4479,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>117</v>
       </c>
@@ -4484,7 +4493,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>117</v>
       </c>
@@ -4498,7 +4507,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>117</v>
       </c>
@@ -4512,7 +4521,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>117</v>
       </c>
@@ -4526,7 +4535,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>127</v>
       </c>
@@ -4540,7 +4549,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>127</v>
       </c>
@@ -4554,7 +4563,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>131</v>
       </c>
@@ -4568,7 +4577,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>131</v>
       </c>
@@ -4582,7 +4591,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>139</v>
       </c>
@@ -4596,7 +4605,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>139</v>
       </c>
@@ -4610,7 +4619,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>139</v>
       </c>
@@ -4624,7 +4633,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>139</v>
       </c>
@@ -4638,7 +4647,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>139</v>
       </c>
@@ -4652,7 +4661,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>139</v>
       </c>
@@ -4666,7 +4675,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>137</v>
       </c>
@@ -4680,7 +4689,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>137</v>
       </c>
@@ -4694,7 +4703,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>137</v>
       </c>
@@ -4708,7 +4717,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>137</v>
       </c>
@@ -4722,7 +4731,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>137</v>
       </c>
@@ -4736,7 +4745,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>137</v>
       </c>
@@ -4750,7 +4759,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>137</v>
       </c>
@@ -4764,7 +4773,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>137</v>
       </c>
@@ -4778,7 +4787,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>147</v>
       </c>
@@ -4792,7 +4801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>147</v>
       </c>
@@ -4806,7 +4815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>151</v>
       </c>
@@ -4820,7 +4829,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>151</v>
       </c>
@@ -4834,7 +4843,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>159</v>
       </c>
@@ -4848,7 +4857,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>159</v>
       </c>
@@ -4862,7 +4871,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>159</v>
       </c>
@@ -4876,7 +4885,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>159</v>
       </c>
@@ -4890,7 +4899,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>159</v>
       </c>
@@ -4904,7 +4913,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>159</v>
       </c>
@@ -4918,7 +4927,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>157</v>
       </c>
@@ -4932,7 +4941,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>157</v>
       </c>
@@ -4946,7 +4955,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>157</v>
       </c>
@@ -4960,7 +4969,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>157</v>
       </c>
@@ -4974,7 +4983,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>157</v>
       </c>
@@ -4988,7 +4997,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>157</v>
       </c>
@@ -5002,7 +5011,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>157</v>
       </c>
@@ -5016,7 +5025,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>157</v>
       </c>
@@ -5030,7 +5039,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>157</v>
       </c>
@@ -5044,7 +5053,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>157</v>
       </c>
@@ -5058,7 +5067,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>157</v>
       </c>
@@ -5072,7 +5081,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>157</v>
       </c>
@@ -5086,7 +5095,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>157</v>
       </c>
@@ -5100,7 +5109,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>157</v>
       </c>
@@ -5114,7 +5123,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>175</v>
       </c>
@@ -5128,7 +5137,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>175</v>
       </c>
@@ -5142,7 +5151,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>175</v>
       </c>
@@ -5156,7 +5165,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>175</v>
       </c>
@@ -5170,7 +5179,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>175</v>
       </c>
@@ -5184,7 +5193,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>175</v>
       </c>
@@ -5198,7 +5207,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>173</v>
       </c>
@@ -5212,7 +5221,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>173</v>
       </c>
@@ -5226,7 +5235,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>173</v>
       </c>
@@ -5240,7 +5249,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>173</v>
       </c>
@@ -5254,7 +5263,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>173</v>
       </c>
@@ -5268,7 +5277,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>173</v>
       </c>
@@ -5282,7 +5291,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>173</v>
       </c>
@@ -5296,7 +5305,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>173</v>
       </c>
@@ -5310,7 +5319,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>173</v>
       </c>
@@ -5324,7 +5333,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>173</v>
       </c>
@@ -5338,7 +5347,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>173</v>
       </c>
@@ -5352,7 +5361,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>173</v>
       </c>
@@ -5366,7 +5375,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>173</v>
       </c>
@@ -5380,7 +5389,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>173</v>
       </c>
@@ -5394,7 +5403,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>173</v>
       </c>
@@ -5408,7 +5417,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>173</v>
       </c>
@@ -5422,7 +5431,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>173</v>
       </c>
@@ -5436,7 +5445,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>191</v>
       </c>
@@ -5450,7 +5459,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>191</v>
       </c>
@@ -5464,7 +5473,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>191</v>
       </c>
@@ -5478,7 +5487,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>191</v>
       </c>
@@ -5492,7 +5501,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>191</v>
       </c>
@@ -5506,7 +5515,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>191</v>
       </c>
@@ -5520,7 +5529,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>189</v>
       </c>
@@ -5534,7 +5543,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>189</v>
       </c>
@@ -5548,7 +5557,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>189</v>
       </c>
@@ -5562,7 +5571,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>189</v>
       </c>
@@ -5576,7 +5585,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>189</v>
       </c>
@@ -5590,7 +5599,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>189</v>
       </c>
@@ -5604,7 +5613,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>189</v>
       </c>
@@ -5618,7 +5627,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>189</v>
       </c>
@@ -5632,7 +5641,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>189</v>
       </c>
@@ -5646,7 +5655,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>189</v>
       </c>
@@ -5660,7 +5669,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>189</v>
       </c>
@@ -5674,7 +5683,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>189</v>
       </c>
@@ -5688,7 +5697,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>189</v>
       </c>
@@ -5702,7 +5711,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>189</v>
       </c>
@@ -5716,7 +5725,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>207</v>
       </c>
@@ -5730,7 +5739,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>207</v>
       </c>
@@ -5744,7 +5753,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>207</v>
       </c>
@@ -5758,7 +5767,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>207</v>
       </c>
@@ -5772,7 +5781,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>207</v>
       </c>
@@ -5786,7 +5795,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>207</v>
       </c>
@@ -5800,7 +5809,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>205</v>
       </c>
@@ -5814,7 +5823,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>205</v>
       </c>
@@ -5828,7 +5837,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>223</v>
       </c>
@@ -5842,7 +5851,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>223</v>
       </c>
@@ -5856,7 +5865,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>223</v>
       </c>
@@ -5870,7 +5879,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>223</v>
       </c>
@@ -5884,7 +5893,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>223</v>
       </c>
@@ -5898,7 +5907,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>223</v>
       </c>
@@ -5912,7 +5921,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>221</v>
       </c>
@@ -5926,7 +5935,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>221</v>
       </c>
@@ -5940,7 +5949,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>221</v>
       </c>
@@ -5954,7 +5963,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>221</v>
       </c>
@@ -5968,7 +5977,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>221</v>
       </c>
@@ -5982,7 +5991,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>221</v>
       </c>
@@ -5996,7 +6005,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>221</v>
       </c>
@@ -6010,7 +6019,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>221</v>
       </c>
@@ -6024,7 +6033,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>221</v>
       </c>
@@ -6038,7 +6047,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>221</v>
       </c>
@@ -6052,7 +6061,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>221</v>
       </c>
@@ -6066,7 +6075,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>221</v>
       </c>
@@ -6080,7 +6089,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>221</v>
       </c>
@@ -6094,7 +6103,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>221</v>
       </c>
@@ -6108,7 +6117,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>221</v>
       </c>
@@ -6122,7 +6131,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>221</v>
       </c>
@@ -6136,7 +6145,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>221</v>
       </c>
@@ -6150,7 +6159,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>221</v>
       </c>
@@ -6164,7 +6173,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>221</v>
       </c>
@@ -6178,7 +6187,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>221</v>
       </c>
@@ -6192,7 +6201,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>221</v>
       </c>
@@ -6206,7 +6215,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>221</v>
       </c>
@@ -6220,7 +6229,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>221</v>
       </c>
@@ -6234,7 +6243,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>221</v>
       </c>
@@ -6248,7 +6257,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>221</v>
       </c>
@@ -6262,7 +6271,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>221</v>
       </c>
@@ -6276,7 +6285,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>221</v>
       </c>
@@ -6290,7 +6299,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>221</v>
       </c>
@@ -6304,7 +6313,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
         <v>221</v>
       </c>
@@ -6318,661 +6327,661 @@
         <v>283</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="B194" s="17">
+      <c r="B194" s="14">
         <v>60</v>
       </c>
-      <c r="C194" s="18" t="b">
+      <c r="C194" s="15" t="b">
         <v>0</v>
       </c>
       <c r="D194" s="9" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A195" s="19" t="s">
+    <row r="195" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="B195" s="20">
-        <v>0</v>
-      </c>
-      <c r="C195" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D195" s="20" t="s">
+      <c r="B195" s="17">
+        <v>0</v>
+      </c>
+      <c r="C195" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D195" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A196" s="19" t="s">
+    <row r="196" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="B196" s="20">
+      <c r="B196" s="17">
         <v>1</v>
       </c>
-      <c r="C196" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D196" s="20" t="s">
+      <c r="C196" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D196" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A197" s="19" t="s">
+    <row r="197" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="B197" s="20">
-        <v>0</v>
-      </c>
-      <c r="C197" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D197" s="20" t="s">
+      <c r="B197" s="17">
+        <v>0</v>
+      </c>
+      <c r="C197" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D197" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A198" s="19" t="s">
+    <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="B198" s="20">
+      <c r="B198" s="17">
         <v>1</v>
       </c>
-      <c r="C198" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D198" s="20" t="s">
+      <c r="C198" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D198" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A199" s="19" t="s">
+    <row r="199" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="B199" s="20">
-        <v>0</v>
-      </c>
-      <c r="C199" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D199" s="20" t="s">
+      <c r="B199" s="17">
+        <v>0</v>
+      </c>
+      <c r="C199" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D199" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="19" t="s">
+    <row r="200" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="B200" s="20">
+      <c r="B200" s="17">
         <v>1</v>
       </c>
-      <c r="C200" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D200" s="20" t="s">
+      <c r="C200" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D200" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A201" s="19" t="s">
+    <row r="201" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="B201" s="20">
-        <v>0</v>
-      </c>
-      <c r="C201" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D201" s="20" t="s">
+      <c r="B201" s="17">
+        <v>0</v>
+      </c>
+      <c r="C201" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D201" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A202" s="19" t="s">
+    <row r="202" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="B202" s="20">
+      <c r="B202" s="17">
         <v>1</v>
       </c>
-      <c r="C202" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D202" s="20" t="s">
+      <c r="C202" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D202" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="19" t="s">
+    <row r="203" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="B203" s="20">
-        <v>0</v>
-      </c>
-      <c r="C203" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D203" s="20" t="s">
+      <c r="B203" s="17">
+        <v>0</v>
+      </c>
+      <c r="C203" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D203" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="19" t="s">
+    <row r="204" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="B204" s="20">
+      <c r="B204" s="17">
         <v>1</v>
       </c>
-      <c r="C204" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D204" s="20" t="s">
+      <c r="C204" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D204" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="19" t="s">
+    <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="B205" s="20">
-        <v>0</v>
-      </c>
-      <c r="C205" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D205" s="20" t="s">
+      <c r="B205" s="17">
+        <v>0</v>
+      </c>
+      <c r="C205" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D205" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A206" s="19" t="s">
+    <row r="206" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="B206" s="20">
+      <c r="B206" s="17">
         <v>1</v>
       </c>
-      <c r="C206" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D206" s="20" t="s">
+      <c r="C206" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D206" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A207" s="19" t="s">
+    <row r="207" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="B207" s="20">
-        <v>0</v>
-      </c>
-      <c r="C207" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D207" s="20" t="s">
+      <c r="B207" s="17">
+        <v>0</v>
+      </c>
+      <c r="C207" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D207" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A208" s="19" t="s">
+    <row r="208" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="B208" s="20">
+      <c r="B208" s="17">
         <v>1</v>
       </c>
-      <c r="C208" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D208" s="20" t="s">
+      <c r="C208" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D208" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A209" s="19" t="s">
+    <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="B209" s="20">
-        <v>0</v>
-      </c>
-      <c r="C209" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D209" s="20" t="s">
+      <c r="B209" s="17">
+        <v>0</v>
+      </c>
+      <c r="C209" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D209" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A210" s="19" t="s">
+    <row r="210" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="B210" s="20">
+      <c r="B210" s="17">
         <v>1</v>
       </c>
-      <c r="C210" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D210" s="20" t="s">
+      <c r="C210" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D210" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A211" s="19" t="s">
+    <row r="211" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="B211" s="20">
-        <v>0</v>
-      </c>
-      <c r="C211" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D211" s="20" t="s">
+      <c r="B211" s="17">
+        <v>0</v>
+      </c>
+      <c r="C211" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D211" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A212" s="19" t="s">
+    <row r="212" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="B212" s="20">
+      <c r="B212" s="17">
         <v>1</v>
       </c>
-      <c r="C212" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D212" s="20" t="s">
+      <c r="C212" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D212" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A213" s="19" t="s">
+    <row r="213" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="B213" s="20">
-        <v>0</v>
-      </c>
-      <c r="C213" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D213" s="20" t="s">
+      <c r="B213" s="17">
+        <v>0</v>
+      </c>
+      <c r="C213" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D213" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="19" t="s">
+    <row r="214" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="B214" s="20">
+      <c r="B214" s="17">
         <v>1</v>
       </c>
-      <c r="C214" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D214" s="20" t="s">
+      <c r="C214" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D214" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A215" s="19" t="s">
+    <row r="215" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="B215" s="20">
-        <v>0</v>
-      </c>
-      <c r="C215" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D215" s="20" t="s">
+      <c r="B215" s="17">
+        <v>0</v>
+      </c>
+      <c r="C215" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D215" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A216" s="19" t="s">
+    <row r="216" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="B216" s="20">
+      <c r="B216" s="17">
         <v>1</v>
       </c>
-      <c r="C216" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D216" s="20" t="s">
+      <c r="C216" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D216" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A217" s="19" t="s">
+    <row r="217" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="B217" s="20">
-        <v>0</v>
-      </c>
-      <c r="C217" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D217" s="20" t="s">
+      <c r="B217" s="17">
+        <v>0</v>
+      </c>
+      <c r="C217" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D217" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A218" s="19" t="s">
+    <row r="218" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="B218" s="20">
+      <c r="B218" s="17">
         <v>1</v>
       </c>
-      <c r="C218" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D218" s="20" t="s">
+      <c r="C218" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D218" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A219" s="19" t="s">
+    <row r="219" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="B219" s="20">
-        <v>0</v>
-      </c>
-      <c r="C219" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D219" s="20" t="s">
+      <c r="B219" s="17">
+        <v>0</v>
+      </c>
+      <c r="C219" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D219" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A220" s="19" t="s">
+    <row r="220" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="B220" s="20">
+      <c r="B220" s="17">
         <v>1</v>
       </c>
-      <c r="C220" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D220" s="20" t="s">
+      <c r="C220" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D220" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A221" s="19" t="s">
+    <row r="221" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="B221" s="20">
-        <v>0</v>
-      </c>
-      <c r="C221" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D221" s="20" t="s">
+      <c r="B221" s="17">
+        <v>0</v>
+      </c>
+      <c r="C221" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D221" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A222" s="19" t="s">
+    <row r="222" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="B222" s="20">
+      <c r="B222" s="17">
         <v>1</v>
       </c>
-      <c r="C222" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D222" s="20" t="s">
+      <c r="C222" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D222" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A223" s="19" t="s">
+    <row r="223" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="B223" s="20">
-        <v>0</v>
-      </c>
-      <c r="C223" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D223" s="20" t="s">
+      <c r="B223" s="17">
+        <v>0</v>
+      </c>
+      <c r="C223" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D223" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A224" s="19" t="s">
+    <row r="224" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="B224" s="20">
+      <c r="B224" s="17">
         <v>1</v>
       </c>
-      <c r="C224" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D224" s="20" t="s">
+      <c r="C224" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D224" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A225" s="19" t="s">
+    <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="B225" s="20">
-        <v>0</v>
-      </c>
-      <c r="C225" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D225" s="20" t="s">
+      <c r="B225" s="17">
+        <v>0</v>
+      </c>
+      <c r="C225" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D225" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A226" s="19" t="s">
+    <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="B226" s="20">
+      <c r="B226" s="17">
         <v>1</v>
       </c>
-      <c r="C226" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D226" s="20" t="s">
+      <c r="C226" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D226" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A227" s="19" t="s">
+    <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="B227" s="20">
-        <v>0</v>
-      </c>
-      <c r="C227" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D227" s="20" t="s">
+      <c r="B227" s="17">
+        <v>0</v>
+      </c>
+      <c r="C227" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D227" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A228" s="19" t="s">
+    <row r="228" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="B228" s="20">
+      <c r="B228" s="17">
         <v>1</v>
       </c>
-      <c r="C228" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D228" s="20" t="s">
+      <c r="C228" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D228" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A229" s="19" t="s">
+    <row r="229" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="B229" s="20">
-        <v>0</v>
-      </c>
-      <c r="C229" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D229" s="20" t="s">
+      <c r="B229" s="17">
+        <v>0</v>
+      </c>
+      <c r="C229" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D229" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A230" s="19" t="s">
+    <row r="230" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="B230" s="20">
+      <c r="B230" s="17">
         <v>1</v>
       </c>
-      <c r="C230" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D230" s="20" t="s">
+      <c r="C230" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D230" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A231" s="19" t="s">
+    <row r="231" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="B231" s="20">
-        <v>0</v>
-      </c>
-      <c r="C231" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D231" s="20" t="s">
+      <c r="B231" s="17">
+        <v>0</v>
+      </c>
+      <c r="C231" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D231" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A232" s="19" t="s">
+    <row r="232" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A232" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="B232" s="20">
+      <c r="B232" s="17">
         <v>1</v>
       </c>
-      <c r="C232" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D232" s="20" t="s">
+      <c r="C232" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D232" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A233" s="19" t="s">
+    <row r="233" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="B233" s="20">
-        <v>0</v>
-      </c>
-      <c r="C233" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D233" s="20" t="s">
+      <c r="B233" s="17">
+        <v>0</v>
+      </c>
+      <c r="C233" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D233" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A234" s="19" t="s">
+    <row r="234" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="B234" s="20">
+      <c r="B234" s="17">
         <v>1</v>
       </c>
-      <c r="C234" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D234" s="20" t="s">
+      <c r="C234" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D234" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A235" s="19" t="s">
+    <row r="235" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="B235" s="20">
-        <v>0</v>
-      </c>
-      <c r="C235" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D235" s="20" t="s">
+      <c r="B235" s="17">
+        <v>0</v>
+      </c>
+      <c r="C235" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D235" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A236" s="19" t="s">
+    <row r="236" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="B236" s="20">
+      <c r="B236" s="17">
         <v>1</v>
       </c>
-      <c r="C236" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D236" s="20" t="s">
+      <c r="C236" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D236" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A237" s="19" t="s">
+    <row r="237" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="B237" s="20">
-        <v>0</v>
-      </c>
-      <c r="C237" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D237" s="20" t="s">
+      <c r="B237" s="17">
+        <v>0</v>
+      </c>
+      <c r="C237" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D237" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A238" s="19" t="s">
+    <row r="238" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="B238" s="20">
+      <c r="B238" s="17">
         <v>1</v>
       </c>
-      <c r="C238" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D238" s="20" t="s">
+      <c r="C238" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D238" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A239" s="19" t="s">
+    <row r="239" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="B239" s="20">
-        <v>0</v>
-      </c>
-      <c r="C239" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D239" s="20" t="s">
+      <c r="B239" s="17">
+        <v>0</v>
+      </c>
+      <c r="C239" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D239" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A240" s="19" t="s">
+    <row r="240" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="B240" s="20">
+      <c r="B240" s="17">
         <v>1</v>
       </c>
-      <c r="C240" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D240" s="20" t="s">
+      <c r="C240" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D240" s="17" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add FEF75_z_ and amend FeNO_
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DEDDF1-4862-5C42-8A86-AD419A4A615D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554BFBDC-628E-D247-8B8A-08A5ACA96393}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="357">
   <si>
     <t>name</t>
   </si>
@@ -1092,6 +1092,12 @@
   </si>
   <si>
     <t>inh_all_sens_SPT_HDM_mix _</t>
+  </si>
+  <si>
+    <t>FEF75_z_</t>
+  </si>
+  <si>
+    <t>FEF75 (z-score according to GLI)</t>
   </si>
 </sst>
 </file>
@@ -1213,13 +1219,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1243,12 +1250,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{FEEDB143-96D9-0349-8C64-FE1E74CAE956}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1707,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG130"/>
+  <dimension ref="A1:BG131"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108:D130"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2033,22 +2048,22 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>55</v>
+      <c r="A19" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>5</v>
@@ -2057,40 +2072,40 @@
         <v>6</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -2099,12 +2114,12 @@
         <v>6</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>5</v>
@@ -2113,12 +2128,12 @@
         <v>6</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>5</v>
@@ -2127,40 +2142,40 @@
         <v>6</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="B27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -2169,124 +2184,124 @@
         <v>17</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>75</v>
+      <c r="D29" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>77</v>
+      <c r="D30" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="11" t="s">
+      <c r="B33" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="B34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>5</v>
@@ -2295,26 +2310,26 @@
         <v>6</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>12</v>
@@ -2323,12 +2338,12 @@
         <v>6</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>12</v>
@@ -2337,12 +2352,12 @@
         <v>6</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>12</v>
@@ -2351,40 +2366,40 @@
         <v>6</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>5</v>
@@ -2393,26 +2408,26 @@
         <v>6</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>12</v>
@@ -2421,12 +2436,12 @@
         <v>6</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>12</v>
@@ -2435,12 +2450,12 @@
         <v>6</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>12</v>
@@ -2449,40 +2464,40 @@
         <v>6</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>5</v>
@@ -2491,26 +2506,26 @@
         <v>6</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>12</v>
@@ -2519,12 +2534,12 @@
         <v>6</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>12</v>
@@ -2533,96 +2548,96 @@
         <v>6</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>5</v>
@@ -2631,26 +2646,26 @@
         <v>6</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C62" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B63" s="11" t="s">
         <v>12</v>
@@ -2659,12 +2674,12 @@
         <v>6</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>12</v>
@@ -2673,96 +2688,96 @@
         <v>6</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C68" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>5</v>
@@ -2771,26 +2786,26 @@
         <v>6</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>12</v>
@@ -2799,12 +2814,12 @@
         <v>6</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>12</v>
@@ -2813,12 +2828,12 @@
         <v>6</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>12</v>
@@ -2827,12 +2842,12 @@
         <v>6</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>12</v>
@@ -2841,40 +2856,40 @@
         <v>6</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>5</v>
@@ -2883,26 +2898,26 @@
         <v>6</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>12</v>
@@ -2911,12 +2926,12 @@
         <v>6</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>12</v>
@@ -2925,12 +2940,12 @@
         <v>6</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B83" s="11" t="s">
         <v>12</v>
@@ -2939,12 +2954,12 @@
         <v>6</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B84" s="11" t="s">
         <v>12</v>
@@ -2953,40 +2968,40 @@
         <v>6</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B87" s="11" t="s">
         <v>5</v>
@@ -2995,26 +3010,26 @@
         <v>6</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C88" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B89" s="11" t="s">
         <v>12</v>
@@ -3023,12 +3038,12 @@
         <v>6</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B90" s="11" t="s">
         <v>12</v>
@@ -3037,12 +3052,12 @@
         <v>6</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>12</v>
@@ -3051,12 +3066,12 @@
         <v>6</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>12</v>
@@ -3065,40 +3080,40 @@
         <v>6</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B93" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B95" s="11" t="s">
         <v>5</v>
@@ -3107,26 +3122,26 @@
         <v>6</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C96" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B97" s="11" t="s">
         <v>12</v>
@@ -3135,12 +3150,12 @@
         <v>6</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B98" s="11" t="s">
         <v>12</v>
@@ -3149,12 +3164,12 @@
         <v>6</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B99" s="11" t="s">
         <v>12</v>
@@ -3163,12 +3178,12 @@
         <v>6</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>12</v>
@@ -3177,40 +3192,40 @@
         <v>6</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B101" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B103" s="11" t="s">
         <v>5</v>
@@ -3219,26 +3234,26 @@
         <v>6</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C104" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B105" s="11" t="s">
         <v>12</v>
@@ -3247,12 +3262,12 @@
         <v>6</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B106" s="11" t="s">
         <v>12</v>
@@ -3261,82 +3276,82 @@
         <v>6</v>
       </c>
       <c r="D106" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="13" t="s">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="B107" s="13" t="s">
+      <c r="B108" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C107" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" s="13" t="s">
+      <c r="C108" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="13" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>303</v>
-      </c>
-      <c r="B108" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" t="s">
-        <v>6</v>
-      </c>
-      <c r="D108" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>303</v>
+      </c>
+      <c r="B109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>305</v>
       </c>
-      <c r="B109" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="18" t="s">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="B110" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" t="s">
-        <v>6</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>309</v>
-      </c>
-      <c r="B111" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>350</v>
+        <v>309</v>
       </c>
       <c r="B112" t="s">
         <v>5</v>
@@ -3345,12 +3360,12 @@
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B113" t="s">
         <v>5</v>
@@ -3359,12 +3374,12 @@
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>315</v>
+        <v>351</v>
       </c>
       <c r="B114" t="s">
         <v>5</v>
@@ -3373,12 +3388,12 @@
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>352</v>
+        <v>315</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
@@ -3387,12 +3402,12 @@
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B116" t="s">
         <v>5</v>
@@ -3401,12 +3416,12 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="B117" t="s">
         <v>5</v>
@@ -3415,12 +3430,12 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
@@ -3429,12 +3444,12 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B119" t="s">
         <v>5</v>
@@ -3443,12 +3458,12 @@
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
@@ -3457,12 +3472,12 @@
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B121" t="s">
         <v>5</v>
@@ -3471,12 +3486,12 @@
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B122" t="s">
         <v>5</v>
@@ -3485,12 +3500,12 @@
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B123" t="s">
         <v>5</v>
@@ -3499,12 +3514,12 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B124" t="s">
         <v>5</v>
@@ -3513,12 +3528,12 @@
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B125" t="s">
         <v>5</v>
@@ -3527,12 +3542,12 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="B126" t="s">
         <v>5</v>
@@ -3541,12 +3556,12 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
@@ -3555,12 +3570,12 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
@@ -3569,12 +3584,12 @@
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
@@ -3583,20 +3598,34 @@
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>345</v>
+      </c>
+      <c r="B130" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>347</v>
       </c>
-      <c r="B130" t="s">
-        <v>5</v>
-      </c>
-      <c r="C130" t="s">
-        <v>6</v>
-      </c>
-      <c r="D130" t="s">
+      <c r="B131" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" t="s">
+        <v>6</v>
+      </c>
+      <c r="D131" t="s">
         <v>348</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: added the asthma variables again
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554BFBDC-628E-D247-8B8A-08A5ACA96393}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55C2EF4-D808-164B-9CA7-62053BD5AB8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="361">
   <si>
     <t>name</t>
   </si>
@@ -1098,6 +1098,18 @@
   </si>
   <si>
     <t>FEF75 (z-score according to GLI)</t>
+  </si>
+  <si>
+    <t>asthma_current_MeDALL_</t>
+  </si>
+  <si>
+    <t>Current asthma (MeDALL)</t>
+  </si>
+  <si>
+    <t>asthma_current_ISAAC_</t>
+  </si>
+  <si>
+    <t>Current asthma  (ISAAC)</t>
   </si>
 </sst>
 </file>
@@ -1722,10 +1734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG131"/>
+  <dimension ref="A1:BG133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1877,7 +1889,7 @@
     </row>
     <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>357</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -1886,114 +1898,116 @@
         <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>31</v>
+        <v>358</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="E10"/>
+    </row>
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E9"/>
-    </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E10"/>
-    </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
@@ -2002,40 +2016,40 @@
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>12</v>
@@ -2044,68 +2058,68 @@
         <v>15</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
-        <v>355</v>
-      </c>
-      <c r="B19" s="20" t="s">
+      <c r="A19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>356</v>
+      <c r="D19" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>57</v>
+      <c r="A21" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -2114,26 +2128,26 @@
         <v>6</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>5</v>
@@ -2142,12 +2156,12 @@
         <v>6</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>5</v>
@@ -2156,68 +2170,68 @@
         <v>6</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="B29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>75</v>
+      <c r="D30" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>12</v>
@@ -2226,138 +2240,138 @@
         <v>17</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="A34" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>83</v>
+      <c r="D34" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>88</v>
+      <c r="A36" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>12</v>
@@ -2366,12 +2380,12 @@
         <v>6</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>12</v>
@@ -2380,82 +2394,82 @@
         <v>6</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>12</v>
@@ -2464,12 +2478,12 @@
         <v>6</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>12</v>
@@ -2478,82 +2492,82 @@
         <v>6</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>12</v>
@@ -2562,40 +2576,40 @@
         <v>6</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>5</v>
@@ -2604,96 +2618,96 @@
         <v>6</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B65" s="11" t="s">
         <v>12</v>
@@ -2702,40 +2716,40 @@
         <v>6</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>5</v>
@@ -2744,96 +2758,96 @@
         <v>6</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C74" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>12</v>
@@ -2842,12 +2856,12 @@
         <v>6</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>12</v>
@@ -2856,12 +2870,12 @@
         <v>6</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>12</v>
@@ -2870,82 +2884,82 @@
         <v>6</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C79" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C81" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B83" s="11" t="s">
         <v>12</v>
@@ -2954,12 +2968,12 @@
         <v>6</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B84" s="11" t="s">
         <v>12</v>
@@ -2968,12 +2982,12 @@
         <v>6</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B85" s="11" t="s">
         <v>12</v>
@@ -2982,82 +2996,82 @@
         <v>6</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B86" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C87" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C89" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C90" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>12</v>
@@ -3066,12 +3080,12 @@
         <v>6</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>12</v>
@@ -3080,12 +3094,12 @@
         <v>6</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B93" s="11" t="s">
         <v>12</v>
@@ -3094,82 +3108,82 @@
         <v>6</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B94" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C95" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C97" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B99" s="11" t="s">
         <v>12</v>
@@ -3178,12 +3192,12 @@
         <v>6</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B100" s="11" t="s">
         <v>12</v>
@@ -3192,12 +3206,12 @@
         <v>6</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B101" s="11" t="s">
         <v>12</v>
@@ -3206,82 +3220,82 @@
         <v>6</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B102" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C103" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C105" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C106" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B107" s="11" t="s">
         <v>12</v>
@@ -3290,68 +3304,68 @@
         <v>6</v>
       </c>
       <c r="D107" s="11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="13" t="s">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="B108" s="13" t="s">
+      <c r="B110" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D108" s="13" t="s">
+      <c r="C110" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" s="13" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>303</v>
       </c>
-      <c r="B109" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>305</v>
-      </c>
-      <c r="B110" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" t="s">
-        <v>6</v>
-      </c>
-      <c r="D110" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="B111" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B112" t="s">
         <v>5</v>
@@ -3360,12 +3374,12 @@
         <v>6</v>
       </c>
       <c r="D112" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>350</v>
+      <c r="A113" s="18" t="s">
+        <v>349</v>
       </c>
       <c r="B113" t="s">
         <v>5</v>
@@ -3374,12 +3388,12 @@
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>351</v>
+        <v>309</v>
       </c>
       <c r="B114" t="s">
         <v>5</v>
@@ -3388,12 +3402,12 @@
         <v>6</v>
       </c>
       <c r="D114" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>315</v>
+        <v>350</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
@@ -3402,12 +3416,12 @@
         <v>6</v>
       </c>
       <c r="D115" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B116" t="s">
         <v>5</v>
@@ -3416,12 +3430,12 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>353</v>
+        <v>315</v>
       </c>
       <c r="B117" t="s">
         <v>5</v>
@@ -3430,12 +3444,12 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>321</v>
+        <v>352</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
@@ -3444,12 +3458,12 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>323</v>
+        <v>353</v>
       </c>
       <c r="B119" t="s">
         <v>5</v>
@@ -3458,12 +3472,12 @@
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
@@ -3472,12 +3486,12 @@
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B121" t="s">
         <v>5</v>
@@ -3486,12 +3500,12 @@
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B122" t="s">
         <v>5</v>
@@ -3500,12 +3514,12 @@
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B123" t="s">
         <v>5</v>
@@ -3514,12 +3528,12 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B124" t="s">
         <v>5</v>
@@ -3528,12 +3542,12 @@
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B125" t="s">
         <v>5</v>
@@ -3542,12 +3556,12 @@
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B126" t="s">
         <v>5</v>
@@ -3556,12 +3570,12 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
@@ -3570,12 +3584,12 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
@@ -3584,12 +3598,12 @@
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
@@ -3598,12 +3612,12 @@
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
@@ -3612,20 +3626,48 @@
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>343</v>
+      </c>
+      <c r="B131" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" t="s">
+        <v>6</v>
+      </c>
+      <c r="D131" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>345</v>
+      </c>
+      <c r="B132" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" t="s">
+        <v>6</v>
+      </c>
+      <c r="D132" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>347</v>
       </c>
-      <c r="B131" t="s">
-        <v>5</v>
-      </c>
-      <c r="C131" t="s">
-        <v>6</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" t="s">
         <v>348</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: added categories as well
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55C2EF4-D808-164B-9CA7-62053BD5AB8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238CCCF7-FACC-9143-B898-25463E167FF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="361">
   <si>
     <t>name</t>
   </si>
@@ -1238,7 +1238,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1269,6 +1269,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1736,7 +1737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -3683,10 +3684,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D240"/>
+  <dimension ref="A1:D244"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A182" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A235" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3865,64 +3866,64 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="B13" s="22">
+        <v>0</v>
+      </c>
+      <c r="C13" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" s="22">
+        <v>1</v>
+      </c>
+      <c r="C14" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="B15" s="22">
+        <v>0</v>
+      </c>
+      <c r="C15" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="B16" s="22">
+        <v>1</v>
+      </c>
+      <c r="C16" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -3935,8 +3936,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>54</v>
+      <c r="A18" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -3949,8 +3950,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>56</v>
+      <c r="A19" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -3963,8 +3964,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>56</v>
+      <c r="A20" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -3978,7 +3979,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -3992,7 +3993,7 @@
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -4006,7 +4007,7 @@
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -4020,7 +4021,7 @@
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -4034,7 +4035,7 @@
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
@@ -4048,7 +4049,7 @@
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
@@ -4062,7 +4063,7 @@
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B27" s="3">
         <v>0</v>
@@ -4076,7 +4077,7 @@
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
@@ -4090,7 +4091,7 @@
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B29" s="3">
         <v>0</v>
@@ -4104,7 +4105,7 @@
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
@@ -4118,58 +4119,58 @@
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B31" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>233</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>234</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="B33" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C33" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>235</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="B34" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>236</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4177,13 +4178,13 @@
         <v>91</v>
       </c>
       <c r="B35" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C35" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4191,69 +4192,69 @@
         <v>91</v>
       </c>
       <c r="B36" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C36" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B37" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C37" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B38" s="3">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C38" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B39" s="3">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C39" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B40" s="3">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C40" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4261,13 +4262,13 @@
         <v>89</v>
       </c>
       <c r="B41" s="3">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C41" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4275,69 +4276,69 @@
         <v>89</v>
       </c>
       <c r="B42" s="3">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="C42" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B43" s="3">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C43" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B44" s="3">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="C44" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B45" s="3">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C45" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B46" s="3">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="C46" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4345,13 +4346,13 @@
         <v>105</v>
       </c>
       <c r="B47" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C47" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4359,69 +4360,69 @@
         <v>105</v>
       </c>
       <c r="B48" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C48" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B49" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C49" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B50" s="3">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C50" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B51" s="3">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C51" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B52" s="3">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C52" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4429,13 +4430,13 @@
         <v>103</v>
       </c>
       <c r="B53" s="3">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C53" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4443,69 +4444,69 @@
         <v>103</v>
       </c>
       <c r="B54" s="3">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="C54" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B55" s="3">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C55" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B56" s="3">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="C56" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B57" s="3">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C57" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B58" s="3">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="C58" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4513,13 +4514,13 @@
         <v>119</v>
       </c>
       <c r="B59" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C59" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4527,69 +4528,69 @@
         <v>119</v>
       </c>
       <c r="B60" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C60" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B61" s="3">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C61" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B62" s="3">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C62" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B63" s="3">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C63" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B64" s="3">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C64" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4597,125 +4598,125 @@
         <v>117</v>
       </c>
       <c r="B65" s="3">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="C65" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B66" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C66" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>18</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B67" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C67" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>19</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B68" s="3">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C68" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B69" s="3">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="C69" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B70" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>233</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B71" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C71" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>234</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B72" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C72" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B73" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C73" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4723,13 +4724,13 @@
         <v>139</v>
       </c>
       <c r="B74" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C74" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4737,69 +4738,69 @@
         <v>139</v>
       </c>
       <c r="B75" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C75" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B76" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C76" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B77" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C77" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B78" s="3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C78" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B79" s="3">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C79" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4807,13 +4808,13 @@
         <v>137</v>
       </c>
       <c r="B80" s="3">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C80" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4821,13 +4822,13 @@
         <v>137</v>
       </c>
       <c r="B81" s="3">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C81" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4835,13 +4836,13 @@
         <v>137</v>
       </c>
       <c r="B82" s="3">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C82" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4849,125 +4850,125 @@
         <v>137</v>
       </c>
       <c r="B83" s="3">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C83" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B84" s="3">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C84" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B85" s="3">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C85" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>19</v>
+        <v>255</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B86" s="3">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C86" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B87" s="3">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C87" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B88" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>233</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B89" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>234</v>
+        <v>19</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B90" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C90" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B91" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C91" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4975,13 +4976,13 @@
         <v>159</v>
       </c>
       <c r="B92" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C92" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4989,32 +4990,32 @@
         <v>159</v>
       </c>
       <c r="B93" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C93" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B94" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C94" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B95" s="3">
         <v>4</v>
@@ -5023,35 +5024,35 @@
         <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B96" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C96" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B97" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C97" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5059,13 +5060,13 @@
         <v>157</v>
       </c>
       <c r="B98" s="3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C98" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5073,13 +5074,13 @@
         <v>157</v>
       </c>
       <c r="B99" s="3">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C99" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5087,13 +5088,13 @@
         <v>157</v>
       </c>
       <c r="B100" s="3">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C100" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5101,13 +5102,13 @@
         <v>157</v>
       </c>
       <c r="B101" s="3">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C101" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5115,13 +5116,13 @@
         <v>157</v>
       </c>
       <c r="B102" s="3">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C102" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5129,13 +5130,13 @@
         <v>157</v>
       </c>
       <c r="B103" s="3">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C103" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5143,13 +5144,13 @@
         <v>157</v>
       </c>
       <c r="B104" s="3">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C104" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5157,13 +5158,13 @@
         <v>157</v>
       </c>
       <c r="B105" s="3">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C105" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5171,13 +5172,13 @@
         <v>157</v>
       </c>
       <c r="B106" s="3">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C106" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5185,69 +5186,69 @@
         <v>157</v>
       </c>
       <c r="B107" s="3">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C107" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B108" s="3">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C108" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>233</v>
+        <v>268</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B109" s="3">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="C109" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>234</v>
+        <v>269</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B110" s="3">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C110" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>235</v>
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B111" s="3">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C111" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>236</v>
+        <v>271</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5255,13 +5256,13 @@
         <v>175</v>
       </c>
       <c r="B112" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C112" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5269,32 +5270,32 @@
         <v>175</v>
       </c>
       <c r="B113" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C113" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B114" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C114" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B115" s="3">
         <v>4</v>
@@ -5303,35 +5304,35 @@
         <v>0</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B116" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C116" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B117" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C117" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5339,13 +5340,13 @@
         <v>173</v>
       </c>
       <c r="B118" s="3">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C118" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5353,13 +5354,13 @@
         <v>173</v>
       </c>
       <c r="B119" s="3">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C119" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5367,13 +5368,13 @@
         <v>173</v>
       </c>
       <c r="B120" s="3">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C120" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5381,13 +5382,13 @@
         <v>173</v>
       </c>
       <c r="B121" s="3">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C121" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5395,13 +5396,13 @@
         <v>173</v>
       </c>
       <c r="B122" s="3">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C122" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5409,13 +5410,13 @@
         <v>173</v>
       </c>
       <c r="B123" s="3">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C123" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5423,13 +5424,13 @@
         <v>173</v>
       </c>
       <c r="B124" s="3">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C124" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5437,13 +5438,13 @@
         <v>173</v>
       </c>
       <c r="B125" s="3">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C125" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5451,13 +5452,13 @@
         <v>173</v>
       </c>
       <c r="B126" s="3">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C126" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5465,13 +5466,13 @@
         <v>173</v>
       </c>
       <c r="B127" s="3">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C127" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5479,13 +5480,13 @@
         <v>173</v>
       </c>
       <c r="B128" s="3">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C128" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5493,13 +5494,13 @@
         <v>173</v>
       </c>
       <c r="B129" s="3">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C129" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5507,69 +5508,69 @@
         <v>173</v>
       </c>
       <c r="B130" s="3">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C130" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="B131" s="3">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C131" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>233</v>
+        <v>274</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="B132" s="3">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="C132" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>234</v>
+        <v>269</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="B133" s="3">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="C133" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="B134" s="3">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C134" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>236</v>
+        <v>271</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5577,13 +5578,13 @@
         <v>191</v>
       </c>
       <c r="B135" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C135" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5591,69 +5592,69 @@
         <v>191</v>
       </c>
       <c r="B136" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C136" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B137" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C137" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B138" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C138" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>276</v>
+        <v>236</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B139" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C139" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B140" s="3">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C140" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>277</v>
+        <v>238</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5661,13 +5662,13 @@
         <v>189</v>
       </c>
       <c r="B141" s="3">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C141" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5675,13 +5676,13 @@
         <v>189</v>
       </c>
       <c r="B142" s="3">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C142" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5689,13 +5690,13 @@
         <v>189</v>
       </c>
       <c r="B143" s="3">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C143" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5703,13 +5704,13 @@
         <v>189</v>
       </c>
       <c r="B144" s="3">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C144" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5717,13 +5718,13 @@
         <v>189</v>
       </c>
       <c r="B145" s="3">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C145" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5731,13 +5732,13 @@
         <v>189</v>
       </c>
       <c r="B146" s="3">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C146" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5745,13 +5746,13 @@
         <v>189</v>
       </c>
       <c r="B147" s="3">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C147" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5759,13 +5760,13 @@
         <v>189</v>
       </c>
       <c r="B148" s="3">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C148" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5773,13 +5774,13 @@
         <v>189</v>
       </c>
       <c r="B149" s="3">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C149" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5787,69 +5788,69 @@
         <v>189</v>
       </c>
       <c r="B150" s="3">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C150" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B151" s="3">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C151" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>233</v>
+        <v>281</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B152" s="3">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C152" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>234</v>
+        <v>282</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B153" s="3">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C153" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>235</v>
+        <v>283</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B154" s="3">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C154" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>236</v>
+        <v>284</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5857,13 +5858,13 @@
         <v>207</v>
       </c>
       <c r="B155" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C155" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5871,97 +5872,97 @@
         <v>207</v>
       </c>
       <c r="B156" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C156" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B157" s="3">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C157" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>285</v>
+        <v>235</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B158" s="3">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C158" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B159" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C159" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B160" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C160" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B161" s="3">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C161" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>235</v>
+        <v>285</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="B162" s="3">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C162" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>236</v>
+        <v>286</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5969,13 +5970,13 @@
         <v>223</v>
       </c>
       <c r="B163" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C163" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5983,69 +5984,69 @@
         <v>223</v>
       </c>
       <c r="B164" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C164" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B165" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C165" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B166" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C166" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>276</v>
+        <v>236</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B167" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C167" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>287</v>
+        <v>237</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B168" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C168" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6053,13 +6054,13 @@
         <v>221</v>
       </c>
       <c r="B169" s="3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C169" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>288</v>
+        <v>258</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6067,13 +6068,13 @@
         <v>221</v>
       </c>
       <c r="B170" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C170" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6081,13 +6082,13 @@
         <v>221</v>
       </c>
       <c r="B171" s="3">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C171" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6095,13 +6096,13 @@
         <v>221</v>
       </c>
       <c r="B172" s="3">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C172" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>290</v>
+        <v>260</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6109,13 +6110,13 @@
         <v>221</v>
       </c>
       <c r="B173" s="3">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C173" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6123,13 +6124,13 @@
         <v>221</v>
       </c>
       <c r="B174" s="3">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C174" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>291</v>
+        <v>261</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6137,13 +6138,13 @@
         <v>221</v>
       </c>
       <c r="B175" s="3">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C175" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6151,13 +6152,13 @@
         <v>221</v>
       </c>
       <c r="B176" s="3">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C176" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6165,13 +6166,13 @@
         <v>221</v>
       </c>
       <c r="B177" s="3">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C177" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>293</v>
+        <v>262</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6179,13 +6180,13 @@
         <v>221</v>
       </c>
       <c r="B178" s="3">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C178" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6193,13 +6194,13 @@
         <v>221</v>
       </c>
       <c r="B179" s="3">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C179" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6207,13 +6208,13 @@
         <v>221</v>
       </c>
       <c r="B180" s="3">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C180" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6221,13 +6222,13 @@
         <v>221</v>
       </c>
       <c r="B181" s="3">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C181" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6235,13 +6236,13 @@
         <v>221</v>
       </c>
       <c r="B182" s="3">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C182" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>266</v>
+        <v>294</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6249,13 +6250,13 @@
         <v>221</v>
       </c>
       <c r="B183" s="3">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C183" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6263,13 +6264,13 @@
         <v>221</v>
       </c>
       <c r="B184" s="3">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C184" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6277,13 +6278,13 @@
         <v>221</v>
       </c>
       <c r="B185" s="3">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C185" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6291,13 +6292,13 @@
         <v>221</v>
       </c>
       <c r="B186" s="3">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C186" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6305,13 +6306,13 @@
         <v>221</v>
       </c>
       <c r="B187" s="3">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C187" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6319,13 +6320,13 @@
         <v>221</v>
       </c>
       <c r="B188" s="3">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C188" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6333,13 +6334,13 @@
         <v>221</v>
       </c>
       <c r="B189" s="3">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C189" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6347,13 +6348,13 @@
         <v>221</v>
       </c>
       <c r="B190" s="3">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C190" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6361,13 +6362,13 @@
         <v>221</v>
       </c>
       <c r="B191" s="3">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C191" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6375,13 +6376,13 @@
         <v>221</v>
       </c>
       <c r="B192" s="3">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C192" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>271</v>
+        <v>300</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6389,88 +6390,88 @@
         <v>221</v>
       </c>
       <c r="B193" s="3">
+        <v>51</v>
+      </c>
+      <c r="C193" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B194" s="3">
+        <v>52</v>
+      </c>
+      <c r="C194" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B195" s="3">
+        <v>57</v>
+      </c>
+      <c r="C195" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B196" s="3">
+        <v>58</v>
+      </c>
+      <c r="C196" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B197" s="3">
         <v>59</v>
       </c>
-      <c r="C193" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D193" s="2" t="s">
+      <c r="C197" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D197" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="10" t="s">
+    <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="B194" s="14">
+      <c r="B198" s="14">
         <v>60</v>
       </c>
-      <c r="C194" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="D194" s="9" t="s">
+      <c r="C198" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D198" s="9" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="B195" s="17">
-        <v>0</v>
-      </c>
-      <c r="C195" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D195" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="B196" s="17">
-        <v>1</v>
-      </c>
-      <c r="C196" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D196" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="B197" s="17">
-        <v>0</v>
-      </c>
-      <c r="C197" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D197" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="B198" s="17">
-        <v>1</v>
-      </c>
-      <c r="C198" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D198" s="17" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="16" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B199" s="17">
         <v>0</v>
@@ -6484,7 +6485,7 @@
     </row>
     <row r="200" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="16" t="s">
-        <v>349</v>
+        <v>303</v>
       </c>
       <c r="B200" s="17">
         <v>1</v>
@@ -6498,7 +6499,7 @@
     </row>
     <row r="201" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B201" s="17">
         <v>0</v>
@@ -6512,7 +6513,7 @@
     </row>
     <row r="202" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B202" s="17">
         <v>1</v>
@@ -6526,7 +6527,7 @@
     </row>
     <row r="203" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="16" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B203" s="17">
         <v>0</v>
@@ -6540,7 +6541,7 @@
     </row>
     <row r="204" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="16" t="s">
-        <v>311</v>
+        <v>349</v>
       </c>
       <c r="B204" s="17">
         <v>1</v>
@@ -6554,7 +6555,7 @@
     </row>
     <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="16" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B205" s="17">
         <v>0</v>
@@ -6568,7 +6569,7 @@
     </row>
     <row r="206" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="16" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B206" s="17">
         <v>1</v>
@@ -6582,7 +6583,7 @@
     </row>
     <row r="207" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="16" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B207" s="17">
         <v>0</v>
@@ -6596,7 +6597,7 @@
     </row>
     <row r="208" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="16" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B208" s="17">
         <v>1</v>
@@ -6610,7 +6611,7 @@
     </row>
     <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="16" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B209" s="17">
         <v>0</v>
@@ -6624,7 +6625,7 @@
     </row>
     <row r="210" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="16" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B210" s="17">
         <v>1</v>
@@ -6638,7 +6639,7 @@
     </row>
     <row r="211" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="16" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B211" s="17">
         <v>0</v>
@@ -6652,7 +6653,7 @@
     </row>
     <row r="212" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="16" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B212" s="17">
         <v>1</v>
@@ -6666,7 +6667,7 @@
     </row>
     <row r="213" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="16" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B213" s="17">
         <v>0</v>
@@ -6680,7 +6681,7 @@
     </row>
     <row r="214" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="16" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B214" s="17">
         <v>1</v>
@@ -6694,7 +6695,7 @@
     </row>
     <row r="215" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B215" s="17">
         <v>0</v>
@@ -6708,7 +6709,7 @@
     </row>
     <row r="216" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B216" s="17">
         <v>1</v>
@@ -6722,7 +6723,7 @@
     </row>
     <row r="217" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="16" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B217" s="17">
         <v>0</v>
@@ -6736,7 +6737,7 @@
     </row>
     <row r="218" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="16" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B218" s="17">
         <v>1</v>
@@ -6750,7 +6751,7 @@
     </row>
     <row r="219" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B219" s="17">
         <v>0</v>
@@ -6764,7 +6765,7 @@
     </row>
     <row r="220" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B220" s="17">
         <v>1</v>
@@ -6778,7 +6779,7 @@
     </row>
     <row r="221" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B221" s="17">
         <v>0</v>
@@ -6792,7 +6793,7 @@
     </row>
     <row r="222" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="16" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B222" s="17">
         <v>1</v>
@@ -6806,7 +6807,7 @@
     </row>
     <row r="223" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B223" s="17">
         <v>0</v>
@@ -6820,7 +6821,7 @@
     </row>
     <row r="224" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B224" s="17">
         <v>1</v>
@@ -6834,7 +6835,7 @@
     </row>
     <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="16" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B225" s="17">
         <v>0</v>
@@ -6848,7 +6849,7 @@
     </row>
     <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="16" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B226" s="17">
         <v>1</v>
@@ -6862,7 +6863,7 @@
     </row>
     <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B227" s="17">
         <v>0</v>
@@ -6876,7 +6877,7 @@
     </row>
     <row r="228" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="16" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B228" s="17">
         <v>1</v>
@@ -6890,7 +6891,7 @@
     </row>
     <row r="229" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="16" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B229" s="17">
         <v>0</v>
@@ -6904,7 +6905,7 @@
     </row>
     <row r="230" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="16" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B230" s="17">
         <v>1</v>
@@ -6918,7 +6919,7 @@
     </row>
     <row r="231" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B231" s="17">
         <v>0</v>
@@ -6932,7 +6933,7 @@
     </row>
     <row r="232" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B232" s="17">
         <v>1</v>
@@ -6946,7 +6947,7 @@
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="16" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B233" s="17">
         <v>0</v>
@@ -6960,7 +6961,7 @@
     </row>
     <row r="234" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="16" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B234" s="17">
         <v>1</v>
@@ -6974,7 +6975,7 @@
     </row>
     <row r="235" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="16" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B235" s="17">
         <v>0</v>
@@ -6988,7 +6989,7 @@
     </row>
     <row r="236" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="16" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B236" s="17">
         <v>1</v>
@@ -7002,7 +7003,7 @@
     </row>
     <row r="237" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B237" s="17">
         <v>0</v>
@@ -7016,7 +7017,7 @@
     </row>
     <row r="238" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="16" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B238" s="17">
         <v>1</v>
@@ -7030,7 +7031,7 @@
     </row>
     <row r="239" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="16" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B239" s="17">
         <v>0</v>
@@ -7044,7 +7045,7 @@
     </row>
     <row r="240" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="16" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B240" s="17">
         <v>1</v>
@@ -7053,6 +7054,62 @@
         <v>0</v>
       </c>
       <c r="D240" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="B241" s="17">
+        <v>0</v>
+      </c>
+      <c r="C241" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D241" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="B242" s="17">
+        <v>1</v>
+      </c>
+      <c r="C242" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D242" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B243" s="17">
+        <v>0</v>
+      </c>
+      <c r="C243" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D243" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B244" s="17">
+        <v>1</v>
+      </c>
+      <c r="C244" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D244" s="17" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: fixed WP5 variables amended wp4 var script
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238CCCF7-FACC-9143-B898-25463E167FF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE3223-C7AD-154F-9B51-100D86CA718A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="367">
   <si>
     <t>name</t>
   </si>
@@ -1110,6 +1110,24 @@
   </si>
   <si>
     <t>Current asthma  (ISAAC)</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_TREE_birch_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_HDM_derp_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_HDM_derf_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_DOG_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_CAT_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_GRASS_tim_</t>
   </si>
 </sst>
 </file>
@@ -1737,8 +1755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG133"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3562,7 +3580,7 @@
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>333</v>
+        <v>366</v>
       </c>
       <c r="B126" t="s">
         <v>5</v>
@@ -3576,7 +3594,7 @@
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
@@ -3590,7 +3608,7 @@
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
@@ -3618,7 +3636,7 @@
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>341</v>
+        <v>363</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
@@ -3632,7 +3650,7 @@
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>343</v>
+        <v>362</v>
       </c>
       <c r="B131" t="s">
         <v>5</v>
@@ -3660,7 +3678,7 @@
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="B133" t="s">
         <v>5</v>
@@ -3686,8 +3704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D244"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A235" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" topLeftCell="A215" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A243" sqref="A243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix: removed test from build and fixed last WP5 var
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE3223-C7AD-154F-9B51-100D86CA718A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79525F91-4A43-004D-A773-CA7D0C2B305C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="368">
   <si>
     <t>name</t>
   </si>
@@ -1128,6 +1128,9 @@
   </si>
   <si>
     <t>inh_all_sens_SPT_GRASS_tim_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_GRASS_mix_</t>
   </si>
 </sst>
 </file>
@@ -1755,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3566,7 +3569,7 @@
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>331</v>
+        <v>367</v>
       </c>
       <c r="B125" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
fix: spaces in dictionaries concerning inh_all_sens_SPT_HDM_mix_ and inh_all_sens_SPT_TREE_mix_
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_yearly_rep.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79525F91-4A43-004D-A773-CA7D0C2B305C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7580D5BD-DA46-104C-8636-AFC24C3DA195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="369">
   <si>
     <t>name</t>
   </si>
@@ -1091,9 +1091,6 @@
     <t>food_all_sens_SPT_SES_</t>
   </si>
   <si>
-    <t>inh_all_sens_SPT_HDM_mix _</t>
-  </si>
-  <si>
     <t>FEF75_z_</t>
   </si>
   <si>
@@ -1131,6 +1128,12 @@
   </si>
   <si>
     <t>inh_all_sens_SPT_GRASS_mix_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_HDM_mix_</t>
+  </si>
+  <si>
+    <t>inh_all_sens_SPT_TREE_mix_</t>
   </si>
 </sst>
 </file>
@@ -1759,7 +1762,7 @@
   <dimension ref="A1:BG133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1911,31 +1914,31 @@
     </row>
     <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>357</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>358</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>359</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>360</v>
       </c>
       <c r="E8"/>
     </row>
@@ -2113,7 +2116,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>12</v>
@@ -2122,7 +2125,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3569,7 +3572,7 @@
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B125" t="s">
         <v>5</v>
@@ -3582,8 +3585,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>366</v>
+      <c r="A126" s="22" t="s">
+        <v>365</v>
       </c>
       <c r="B126" t="s">
         <v>5</v>
@@ -3597,7 +3600,7 @@
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
@@ -3611,7 +3614,7 @@
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
@@ -3624,8 +3627,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>354</v>
+      <c r="A129" s="22" t="s">
+        <v>367</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
@@ -3639,7 +3642,7 @@
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
@@ -3652,8 +3655,8 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>362</v>
+      <c r="A131" s="22" t="s">
+        <v>361</v>
       </c>
       <c r="B131" t="s">
         <v>5</v>
@@ -3666,8 +3669,8 @@
       </c>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>345</v>
+      <c r="A132" s="22" t="s">
+        <v>368</v>
       </c>
       <c r="B132" t="s">
         <v>5</v>
@@ -3681,7 +3684,7 @@
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B133" t="s">
         <v>5</v>
@@ -3888,7 +3891,7 @@
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B13" s="22">
         <v>0</v>
@@ -3902,7 +3905,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B14" s="22">
         <v>1</v>
@@ -3916,7 +3919,7 @@
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B15" s="22">
         <v>0</v>
@@ -3930,7 +3933,7 @@
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B16" s="22">
         <v>1</v>

</xml_diff>